<commit_message>
feat: answering more questions
</commit_message>
<xml_diff>
--- a/Data/Climat.xlsx
+++ b/Data/Climat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugotomasi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francoisnicot/Desktop/NF Consulting/cours/cours de référence/qualites données/dataQualite_TP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AB9E82-6EA7-CD43-8036-BD12A6CC710A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C7F7F5-345A-9C47-8277-71AD669EC95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SI " sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
   <si>
     <t>janvier</t>
   </si>
@@ -179,6 +179,9 @@
     <t>min /max</t>
   </si>
   <si>
+    <t>0xFFFF</t>
+  </si>
+  <si>
     <t>identifier les valeurs atypiques ou manquantes</t>
   </si>
   <si>
@@ -222,6 +225,9 @@
   </si>
   <si>
     <t>implémenter ces lois dans votre application précédente</t>
+  </si>
+  <si>
+    <t>Cloudy</t>
   </si>
 </sst>
 </file>
@@ -359,78 +365,78 @@
     </xf>
   </cellXfs>
   <cellStyles count="73">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -778,7 +784,7 @@
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
@@ -2080,7 +2086,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2088,7 +2094,7 @@
         <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -2096,7 +2102,7 @@
         <v>46</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2104,37 +2110,37 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2152,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2519,8 +2525,8 @@
       <c r="L12">
         <v>11</v>
       </c>
-      <c r="M12" s="2">
-        <v>3.5</v>
+      <c r="M12" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="N12">
         <v>5</v>
@@ -2589,9 +2595,8 @@
       <c r="H14">
         <v>5</v>
       </c>
-      <c r="I14">
-        <f>14</f>
-        <v>14</v>
+      <c r="I14" t="s">
+        <v>63</v>
       </c>
       <c r="J14">
         <v>15</v>
@@ -2828,9 +2833,8 @@
       <c r="E20">
         <v>-9</v>
       </c>
-      <c r="F20" s="2">
-        <f>1+3.5</f>
-        <v>4.5</v>
+      <c r="F20" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="G20">
         <v>8</v>
@@ -3129,8 +3133,8 @@
       <c r="I27">
         <v>20</v>
       </c>
-      <c r="J27" s="2">
-        <v>21.5</v>
+      <c r="J27" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="K27">
         <v>17</v>
@@ -3464,18 +3468,18 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
         <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -3483,7 +3487,7 @@
         <v>46</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -3491,47 +3495,47 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>